<commit_message>
Correction of benchmark metrics.
</commit_message>
<xml_diff>
--- a/Benchmark-Ergebnisse.xlsx
+++ b/Benchmark-Ergebnisse.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Google Drive\FHDW_Masterstudium\4_Semester\Seminar zu ausgewählten Forschungsthemen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\Documents\workspaces\seminar_zu_ausgewählten_forschungsthemen\java-frameworks-performance-benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69423AA2-6C0D-42FB-9C08-C70F073A1DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650BA4EC-731C-4B05-B7D9-2E343AE7E34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8745" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -148,27 +147,6 @@
     <t>4. Testzeit in Sekunden</t>
   </si>
   <si>
-    <t>5. Startzeit im DEV-Mode in Millisekunden</t>
-  </si>
-  <si>
-    <t>6. Startzeit im Prod-Mode (denaturiert) in Millisekunden</t>
-  </si>
-  <si>
-    <t>7. Startzeit im Prod-Mode (nativ)  in Millisekunden</t>
-  </si>
-  <si>
-    <t>8. Zeit bis zum ersten Response nach Startup (denaturiert) in Millisekunden</t>
-  </si>
-  <si>
-    <t>9. Zeit bis zum ersten Response nach Startup (nativ) in Millisekunden</t>
-  </si>
-  <si>
-    <t>10. Beantwortete Requests pro Sekunde  (denaturiert)</t>
-  </si>
-  <si>
-    <t>11. Beantwortete Requests pro Sekunde  (nativ)</t>
-  </si>
-  <si>
     <t>12. Memory-Verbrauch ohne Last (denaturiert) in MB</t>
   </si>
   <si>
@@ -185,6 +163,27 @@
   </si>
   <si>
     <t>java -Xmx128m -jar target/…; ab -k -c 20 -n 100000 [url]</t>
+  </si>
+  <si>
+    <t>5. Startzeit im DEV-Mode in Sekunden</t>
+  </si>
+  <si>
+    <t>6. Startzeit im Prod-Mode (denaturiert) in Sekunden</t>
+  </si>
+  <si>
+    <t>7. Startzeit im Prod-Mode (nativ)  in Sekunden</t>
+  </si>
+  <si>
+    <t>8. Zeit bis zum ersten Response nach Startup (denaturiert) in Sekunden</t>
+  </si>
+  <si>
+    <t>9. Zeit bis zum ersten Response nach Startup (nativ) in Sekunden</t>
+  </si>
+  <si>
+    <t>10. Beantwortete Requests pro Sekunde (denaturiert)</t>
+  </si>
+  <si>
+    <t>11. Beantwortete Requests pro Sekunde (nativ)</t>
   </si>
 </sst>
 </file>
@@ -589,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1259,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -1415,7 +1414,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1570,7 +1569,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1725,7 +1724,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1880,7 +1879,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -2025,7 +2024,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -2067,7 +2066,7 @@
         <v>39325.800000000003</v>
       </c>
       <c r="M48" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N48" t="s">
         <v>16</v>
@@ -2112,7 +2111,7 @@
         <v>43057.2</v>
       </c>
       <c r="M49" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N49" t="s">
         <v>26</v>
@@ -2157,7 +2156,7 @@
         <v>47908.1</v>
       </c>
       <c r="M50" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N50" t="s">
         <v>27</v>
@@ -2168,7 +2167,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="L52" s="8"/>
     </row>
@@ -2211,7 +2210,7 @@
         <v>16847.2</v>
       </c>
       <c r="M53" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="N53" t="s">
         <v>23</v>
@@ -2256,7 +2255,7 @@
         <v>13452.9</v>
       </c>
       <c r="M54" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N54" t="s">
         <v>25</v>
@@ -2301,12 +2300,12 @@
         <v>17942.3</v>
       </c>
       <c r="M55" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -2341,7 +2340,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -2370,7 +2369,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -2408,7 +2407,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>